<commit_message>
changes o structure before meeting
</commit_message>
<xml_diff>
--- a/A8 - Self and Peer Assessment /New Self and Peer Assessment Spreadsheet.xlsx
+++ b/A8 - Self and Peer Assessment /New Self and Peer Assessment Spreadsheet.xlsx
@@ -37,28 +37,28 @@
     <t xml:space="preserve">Team Members (Including yourself - alphabetically by surname)</t>
   </si>
   <si>
+    <t xml:space="preserve">Jeremy Ryan Garside</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antonis Georgiou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walid Graihim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haytham Grari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zaham Haider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cameron Haynes</t>
+  </si>
+  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">Contribution Score: Out Of 100%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jeremy Ryan Garside</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antonis Georgiou</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Walid Graihim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Haytham Grari</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zaham Haider</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cameron Haynes</t>
   </si>
   <si>
     <t xml:space="preserve">Total of Contribtions Scores: </t>
@@ -74,7 +74,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -112,24 +112,19 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="DM Sans"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="DM Sans"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,7 +135,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -201,13 +196,6 @@
       <left/>
       <right style="thin"/>
       <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right/>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -258,7 +246,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -307,15 +295,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -323,35 +319,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -547,15 +531,15 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -611,87 +595,87 @@
       <c r="M5" s="10"/>
       <c r="N5" s="11"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="14" t="s">
+    <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="12" t="s">
         <v>5</v>
       </c>
+      <c r="C6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="16" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16" t="n">
+      <c r="A7" s="17"/>
+      <c r="B7" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="17" t="n">
+      <c r="C7" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="D7" s="17" t="n">
+      <c r="D7" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="E7" s="17" t="n">
+      <c r="E7" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="F7" s="17" t="n">
+      <c r="F7" s="19" t="n">
         <v>5</v>
       </c>
-      <c r="G7" s="17" t="n">
+      <c r="G7" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="H7" s="17" t="n">
+      <c r="H7" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="I7" s="17" t="n">
+      <c r="I7" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="J7" s="17" t="n">
+      <c r="J7" s="19" t="n">
         <v>9</v>
       </c>
-      <c r="K7" s="17" t="n">
+      <c r="K7" s="19" t="n">
         <v>10</v>
       </c>
-      <c r="L7" s="17" t="n">
+      <c r="L7" s="19" t="n">
         <v>11</v>
       </c>
-      <c r="M7" s="17" t="n">
+      <c r="M7" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="N7" s="18" t="n">
+      <c r="N7" s="20" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="6" t="s">
+      <c r="A8" s="21" t="s">
         <v>12</v>
       </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
@@ -701,23 +685,23 @@
       <c r="N8" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K10" s="23" t="s">
+      <c r="K10" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
       <c r="N10" s="8" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J12" s="23" t="s">
+      <c r="J12" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>